<commit_message>
ITO-000 create endpoint contest-001, 002
</commit_message>
<xml_diff>
--- a/document/contest-endpoint.xlsx
+++ b/document/contest-endpoint.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="3465" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="3465" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
   <si>
     <t>Context path</t>
   </si>
@@ -33,40 +33,25 @@
     <t>Produce</t>
   </si>
   <si>
-    <t>/onlinejudge-ms-user</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>Require field</t>
   </si>
   <si>
-    <t>/users</t>
-  </si>
-  <si>
     <t>Post</t>
   </si>
   <si>
     <t>JSON</t>
   </si>
   <si>
-    <t>Create new User -&gt; User registration</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
-    <t>#001</t>
-  </si>
-  <si>
     <t>Data- DataModel</t>
   </si>
   <si>
     <t>Data-RequestBody</t>
-  </si>
-  <si>
-    <t>onlinejudge.domain.User</t>
   </si>
   <si>
     <t>Response - DataModel</t>
@@ -204,7 +189,55 @@
     <t>List&lt;Problem&gt;</t>
   </si>
   <si>
-    <t>Get all problem was created by current user</t>
+    <t>Get all problem was created by current user login</t>
+  </si>
+  <si>
+    <t>/onlinejudge-ms-contest</t>
+  </si>
+  <si>
+    <t>#contest-001</t>
+  </si>
+  <si>
+    <t>/contests</t>
+  </si>
+  <si>
+    <t>onlinejudge.domain.Contest</t>
+  </si>
+  <si>
+    <t>Create success</t>
+  </si>
+  <si>
+    <t>contest.001.dataempty</t>
+  </si>
+  <si>
+    <t>Data must not empty</t>
+  </si>
+  <si>
+    <t>Create new Contest or update exist Contest</t>
+  </si>
+  <si>
+    <t>contest.002.fieldempty</t>
+  </si>
+  <si>
+    <t>Some field is empty</t>
+  </si>
+  <si>
+    <t>Data is empty</t>
+  </si>
+  <si>
+    <t>Field {0} must not empty.</t>
+  </si>
+  <si>
+    <t>#contest-002</t>
+  </si>
+  <si>
+    <t>Get all Contest belong to currect user login (admin of contest)</t>
+  </si>
+  <si>
+    <t>/contest</t>
+  </si>
+  <si>
+    <t>List&lt;onlinejudge.domain.Contest&gt;</t>
   </si>
 </sst>
 </file>
@@ -246,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -264,16 +297,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -282,13 +324,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,24 +650,24 @@
   <sheetData>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -635,96 +677,1198 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L6"/>
+  <dimension ref="A3:XFB9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1"/>
     <col min="3" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="7" width="23.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" customWidth="1"/>
+    <col min="7" max="8" width="28.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="23.5703125" customWidth="1"/>
     <col min="11" max="11" width="23.28515625" customWidth="1"/>
-    <col min="12" max="12" width="47.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="35.42578125" customWidth="1"/>
+    <col min="13" max="13" width="35.5703125" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" customWidth="1"/>
+    <col min="15" max="15" width="23.7109375" customWidth="1"/>
+    <col min="16" max="16" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1022 1038:2046 2062:3070 3086:4094 4110:5118 5134:6142 6158:7166 7182:8190 8206:9214 9230:10238 10254:11262 11278:12286 12302:13310 13326:14334 14350:15358 15374:16382" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1022 1038:2046 2062:3070 3086:4094 4110:5118 5134:6142 6158:7166 7182:8190 8206:9214 9230:10238 10254:11262 11278:12286 12302:13310 13326:14334 14350:15358 15374:16382" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="M5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD5" s="5"/>
+      <c r="AT5" s="5"/>
+      <c r="BJ5" s="5"/>
+      <c r="BZ5" s="5"/>
+      <c r="CP5" s="5"/>
+      <c r="DF5" s="5"/>
+      <c r="DV5" s="5"/>
+      <c r="EL5" s="5"/>
+      <c r="FB5" s="5"/>
+      <c r="FR5" s="5"/>
+      <c r="GH5" s="5"/>
+      <c r="GX5" s="5"/>
+      <c r="HN5" s="5"/>
+      <c r="ID5" s="5"/>
+      <c r="IT5" s="5"/>
+      <c r="JJ5" s="5"/>
+      <c r="JZ5" s="5"/>
+      <c r="KP5" s="5"/>
+      <c r="LF5" s="5"/>
+      <c r="LV5" s="5"/>
+      <c r="ML5" s="5"/>
+      <c r="NB5" s="5"/>
+      <c r="NR5" s="5"/>
+      <c r="OH5" s="5"/>
+      <c r="OX5" s="5"/>
+      <c r="PN5" s="5"/>
+      <c r="QD5" s="5"/>
+      <c r="QT5" s="5"/>
+      <c r="RJ5" s="5"/>
+      <c r="RZ5" s="5"/>
+      <c r="SP5" s="5"/>
+      <c r="TF5" s="5"/>
+      <c r="TV5" s="5"/>
+      <c r="UL5" s="5"/>
+      <c r="VB5" s="5"/>
+      <c r="VR5" s="5"/>
+      <c r="WH5" s="5"/>
+      <c r="WX5" s="5"/>
+      <c r="XN5" s="5"/>
+      <c r="YD5" s="5"/>
+      <c r="YT5" s="5"/>
+      <c r="ZJ5" s="5"/>
+      <c r="ZZ5" s="5"/>
+      <c r="AAP5" s="5"/>
+      <c r="ABF5" s="5"/>
+      <c r="ABV5" s="5"/>
+      <c r="ACL5" s="5"/>
+      <c r="ADB5" s="5"/>
+      <c r="ADR5" s="5"/>
+      <c r="AEH5" s="5"/>
+      <c r="AEX5" s="5"/>
+      <c r="AFN5" s="5"/>
+      <c r="AGD5" s="5"/>
+      <c r="AGT5" s="5"/>
+      <c r="AHJ5" s="5"/>
+      <c r="AHZ5" s="5"/>
+      <c r="AIP5" s="5"/>
+      <c r="AJF5" s="5"/>
+      <c r="AJV5" s="5"/>
+      <c r="AKL5" s="5"/>
+      <c r="ALB5" s="5"/>
+      <c r="ALR5" s="5"/>
+      <c r="AMH5" s="5"/>
+      <c r="AMX5" s="5"/>
+      <c r="ANN5" s="5"/>
+      <c r="AOD5" s="5"/>
+      <c r="AOT5" s="5"/>
+      <c r="APJ5" s="5"/>
+      <c r="APZ5" s="5"/>
+      <c r="AQP5" s="5"/>
+      <c r="ARF5" s="5"/>
+      <c r="ARV5" s="5"/>
+      <c r="ASL5" s="5"/>
+      <c r="ATB5" s="5"/>
+      <c r="ATR5" s="5"/>
+      <c r="AUH5" s="5"/>
+      <c r="AUX5" s="5"/>
+      <c r="AVN5" s="5"/>
+      <c r="AWD5" s="5"/>
+      <c r="AWT5" s="5"/>
+      <c r="AXJ5" s="5"/>
+      <c r="AXZ5" s="5"/>
+      <c r="AYP5" s="5"/>
+      <c r="AZF5" s="5"/>
+      <c r="AZV5" s="5"/>
+      <c r="BAL5" s="5"/>
+      <c r="BBB5" s="5"/>
+      <c r="BBR5" s="5"/>
+      <c r="BCH5" s="5"/>
+      <c r="BCX5" s="5"/>
+      <c r="BDN5" s="5"/>
+      <c r="BED5" s="5"/>
+      <c r="BET5" s="5"/>
+      <c r="BFJ5" s="5"/>
+      <c r="BFZ5" s="5"/>
+      <c r="BGP5" s="5"/>
+      <c r="BHF5" s="5"/>
+      <c r="BHV5" s="5"/>
+      <c r="BIL5" s="5"/>
+      <c r="BJB5" s="5"/>
+      <c r="BJR5" s="5"/>
+      <c r="BKH5" s="5"/>
+      <c r="BKX5" s="5"/>
+      <c r="BLN5" s="5"/>
+      <c r="BMD5" s="5"/>
+      <c r="BMT5" s="5"/>
+      <c r="BNJ5" s="5"/>
+      <c r="BNZ5" s="5"/>
+      <c r="BOP5" s="5"/>
+      <c r="BPF5" s="5"/>
+      <c r="BPV5" s="5"/>
+      <c r="BQL5" s="5"/>
+      <c r="BRB5" s="5"/>
+      <c r="BRR5" s="5"/>
+      <c r="BSH5" s="5"/>
+      <c r="BSX5" s="5"/>
+      <c r="BTN5" s="5"/>
+      <c r="BUD5" s="5"/>
+      <c r="BUT5" s="5"/>
+      <c r="BVJ5" s="5"/>
+      <c r="BVZ5" s="5"/>
+      <c r="BWP5" s="5"/>
+      <c r="BXF5" s="5"/>
+      <c r="BXV5" s="5"/>
+      <c r="BYL5" s="5"/>
+      <c r="BZB5" s="5"/>
+      <c r="BZR5" s="5"/>
+      <c r="CAH5" s="5"/>
+      <c r="CAX5" s="5"/>
+      <c r="CBN5" s="5"/>
+      <c r="CCD5" s="5"/>
+      <c r="CCT5" s="5"/>
+      <c r="CDJ5" s="5"/>
+      <c r="CDZ5" s="5"/>
+      <c r="CEP5" s="5"/>
+      <c r="CFF5" s="5"/>
+      <c r="CFV5" s="5"/>
+      <c r="CGL5" s="5"/>
+      <c r="CHB5" s="5"/>
+      <c r="CHR5" s="5"/>
+      <c r="CIH5" s="5"/>
+      <c r="CIX5" s="5"/>
+      <c r="CJN5" s="5"/>
+      <c r="CKD5" s="5"/>
+      <c r="CKT5" s="5"/>
+      <c r="CLJ5" s="5"/>
+      <c r="CLZ5" s="5"/>
+      <c r="CMP5" s="5"/>
+      <c r="CNF5" s="5"/>
+      <c r="CNV5" s="5"/>
+      <c r="COL5" s="5"/>
+      <c r="CPB5" s="5"/>
+      <c r="CPR5" s="5"/>
+      <c r="CQH5" s="5"/>
+      <c r="CQX5" s="5"/>
+      <c r="CRN5" s="5"/>
+      <c r="CSD5" s="5"/>
+      <c r="CST5" s="5"/>
+      <c r="CTJ5" s="5"/>
+      <c r="CTZ5" s="5"/>
+      <c r="CUP5" s="5"/>
+      <c r="CVF5" s="5"/>
+      <c r="CVV5" s="5"/>
+      <c r="CWL5" s="5"/>
+      <c r="CXB5" s="5"/>
+      <c r="CXR5" s="5"/>
+      <c r="CYH5" s="5"/>
+      <c r="CYX5" s="5"/>
+      <c r="CZN5" s="5"/>
+      <c r="DAD5" s="5"/>
+      <c r="DAT5" s="5"/>
+      <c r="DBJ5" s="5"/>
+      <c r="DBZ5" s="5"/>
+      <c r="DCP5" s="5"/>
+      <c r="DDF5" s="5"/>
+      <c r="DDV5" s="5"/>
+      <c r="DEL5" s="5"/>
+      <c r="DFB5" s="5"/>
+      <c r="DFR5" s="5"/>
+      <c r="DGH5" s="5"/>
+      <c r="DGX5" s="5"/>
+      <c r="DHN5" s="5"/>
+      <c r="DID5" s="5"/>
+      <c r="DIT5" s="5"/>
+      <c r="DJJ5" s="5"/>
+      <c r="DJZ5" s="5"/>
+      <c r="DKP5" s="5"/>
+      <c r="DLF5" s="5"/>
+      <c r="DLV5" s="5"/>
+      <c r="DML5" s="5"/>
+      <c r="DNB5" s="5"/>
+      <c r="DNR5" s="5"/>
+      <c r="DOH5" s="5"/>
+      <c r="DOX5" s="5"/>
+      <c r="DPN5" s="5"/>
+      <c r="DQD5" s="5"/>
+      <c r="DQT5" s="5"/>
+      <c r="DRJ5" s="5"/>
+      <c r="DRZ5" s="5"/>
+      <c r="DSP5" s="5"/>
+      <c r="DTF5" s="5"/>
+      <c r="DTV5" s="5"/>
+      <c r="DUL5" s="5"/>
+      <c r="DVB5" s="5"/>
+      <c r="DVR5" s="5"/>
+      <c r="DWH5" s="5"/>
+      <c r="DWX5" s="5"/>
+      <c r="DXN5" s="5"/>
+      <c r="DYD5" s="5"/>
+      <c r="DYT5" s="5"/>
+      <c r="DZJ5" s="5"/>
+      <c r="DZZ5" s="5"/>
+      <c r="EAP5" s="5"/>
+      <c r="EBF5" s="5"/>
+      <c r="EBV5" s="5"/>
+      <c r="ECL5" s="5"/>
+      <c r="EDB5" s="5"/>
+      <c r="EDR5" s="5"/>
+      <c r="EEH5" s="5"/>
+      <c r="EEX5" s="5"/>
+      <c r="EFN5" s="5"/>
+      <c r="EGD5" s="5"/>
+      <c r="EGT5" s="5"/>
+      <c r="EHJ5" s="5"/>
+      <c r="EHZ5" s="5"/>
+      <c r="EIP5" s="5"/>
+      <c r="EJF5" s="5"/>
+      <c r="EJV5" s="5"/>
+      <c r="EKL5" s="5"/>
+      <c r="ELB5" s="5"/>
+      <c r="ELR5" s="5"/>
+      <c r="EMH5" s="5"/>
+      <c r="EMX5" s="5"/>
+      <c r="ENN5" s="5"/>
+      <c r="EOD5" s="5"/>
+      <c r="EOT5" s="5"/>
+      <c r="EPJ5" s="5"/>
+      <c r="EPZ5" s="5"/>
+      <c r="EQP5" s="5"/>
+      <c r="ERF5" s="5"/>
+      <c r="ERV5" s="5"/>
+      <c r="ESL5" s="5"/>
+      <c r="ETB5" s="5"/>
+      <c r="ETR5" s="5"/>
+      <c r="EUH5" s="5"/>
+      <c r="EUX5" s="5"/>
+      <c r="EVN5" s="5"/>
+      <c r="EWD5" s="5"/>
+      <c r="EWT5" s="5"/>
+      <c r="EXJ5" s="5"/>
+      <c r="EXZ5" s="5"/>
+      <c r="EYP5" s="5"/>
+      <c r="EZF5" s="5"/>
+      <c r="EZV5" s="5"/>
+      <c r="FAL5" s="5"/>
+      <c r="FBB5" s="5"/>
+      <c r="FBR5" s="5"/>
+      <c r="FCH5" s="5"/>
+      <c r="FCX5" s="5"/>
+      <c r="FDN5" s="5"/>
+      <c r="FED5" s="5"/>
+      <c r="FET5" s="5"/>
+      <c r="FFJ5" s="5"/>
+      <c r="FFZ5" s="5"/>
+      <c r="FGP5" s="5"/>
+      <c r="FHF5" s="5"/>
+      <c r="FHV5" s="5"/>
+      <c r="FIL5" s="5"/>
+      <c r="FJB5" s="5"/>
+      <c r="FJR5" s="5"/>
+      <c r="FKH5" s="5"/>
+      <c r="FKX5" s="5"/>
+      <c r="FLN5" s="5"/>
+      <c r="FMD5" s="5"/>
+      <c r="FMT5" s="5"/>
+      <c r="FNJ5" s="5"/>
+      <c r="FNZ5" s="5"/>
+      <c r="FOP5" s="5"/>
+      <c r="FPF5" s="5"/>
+      <c r="FPV5" s="5"/>
+      <c r="FQL5" s="5"/>
+      <c r="FRB5" s="5"/>
+      <c r="FRR5" s="5"/>
+      <c r="FSH5" s="5"/>
+      <c r="FSX5" s="5"/>
+      <c r="FTN5" s="5"/>
+      <c r="FUD5" s="5"/>
+      <c r="FUT5" s="5"/>
+      <c r="FVJ5" s="5"/>
+      <c r="FVZ5" s="5"/>
+      <c r="FWP5" s="5"/>
+      <c r="FXF5" s="5"/>
+      <c r="FXV5" s="5"/>
+      <c r="FYL5" s="5"/>
+      <c r="FZB5" s="5"/>
+      <c r="FZR5" s="5"/>
+      <c r="GAH5" s="5"/>
+      <c r="GAX5" s="5"/>
+      <c r="GBN5" s="5"/>
+      <c r="GCD5" s="5"/>
+      <c r="GCT5" s="5"/>
+      <c r="GDJ5" s="5"/>
+      <c r="GDZ5" s="5"/>
+      <c r="GEP5" s="5"/>
+      <c r="GFF5" s="5"/>
+      <c r="GFV5" s="5"/>
+      <c r="GGL5" s="5"/>
+      <c r="GHB5" s="5"/>
+      <c r="GHR5" s="5"/>
+      <c r="GIH5" s="5"/>
+      <c r="GIX5" s="5"/>
+      <c r="GJN5" s="5"/>
+      <c r="GKD5" s="5"/>
+      <c r="GKT5" s="5"/>
+      <c r="GLJ5" s="5"/>
+      <c r="GLZ5" s="5"/>
+      <c r="GMP5" s="5"/>
+      <c r="GNF5" s="5"/>
+      <c r="GNV5" s="5"/>
+      <c r="GOL5" s="5"/>
+      <c r="GPB5" s="5"/>
+      <c r="GPR5" s="5"/>
+      <c r="GQH5" s="5"/>
+      <c r="GQX5" s="5"/>
+      <c r="GRN5" s="5"/>
+      <c r="GSD5" s="5"/>
+      <c r="GST5" s="5"/>
+      <c r="GTJ5" s="5"/>
+      <c r="GTZ5" s="5"/>
+      <c r="GUP5" s="5"/>
+      <c r="GVF5" s="5"/>
+      <c r="GVV5" s="5"/>
+      <c r="GWL5" s="5"/>
+      <c r="GXB5" s="5"/>
+      <c r="GXR5" s="5"/>
+      <c r="GYH5" s="5"/>
+      <c r="GYX5" s="5"/>
+      <c r="GZN5" s="5"/>
+      <c r="HAD5" s="5"/>
+      <c r="HAT5" s="5"/>
+      <c r="HBJ5" s="5"/>
+      <c r="HBZ5" s="5"/>
+      <c r="HCP5" s="5"/>
+      <c r="HDF5" s="5"/>
+      <c r="HDV5" s="5"/>
+      <c r="HEL5" s="5"/>
+      <c r="HFB5" s="5"/>
+      <c r="HFR5" s="5"/>
+      <c r="HGH5" s="5"/>
+      <c r="HGX5" s="5"/>
+      <c r="HHN5" s="5"/>
+      <c r="HID5" s="5"/>
+      <c r="HIT5" s="5"/>
+      <c r="HJJ5" s="5"/>
+      <c r="HJZ5" s="5"/>
+      <c r="HKP5" s="5"/>
+      <c r="HLF5" s="5"/>
+      <c r="HLV5" s="5"/>
+      <c r="HML5" s="5"/>
+      <c r="HNB5" s="5"/>
+      <c r="HNR5" s="5"/>
+      <c r="HOH5" s="5"/>
+      <c r="HOX5" s="5"/>
+      <c r="HPN5" s="5"/>
+      <c r="HQD5" s="5"/>
+      <c r="HQT5" s="5"/>
+      <c r="HRJ5" s="5"/>
+      <c r="HRZ5" s="5"/>
+      <c r="HSP5" s="5"/>
+      <c r="HTF5" s="5"/>
+      <c r="HTV5" s="5"/>
+      <c r="HUL5" s="5"/>
+      <c r="HVB5" s="5"/>
+      <c r="HVR5" s="5"/>
+      <c r="HWH5" s="5"/>
+      <c r="HWX5" s="5"/>
+      <c r="HXN5" s="5"/>
+      <c r="HYD5" s="5"/>
+      <c r="HYT5" s="5"/>
+      <c r="HZJ5" s="5"/>
+      <c r="HZZ5" s="5"/>
+      <c r="IAP5" s="5"/>
+      <c r="IBF5" s="5"/>
+      <c r="IBV5" s="5"/>
+      <c r="ICL5" s="5"/>
+      <c r="IDB5" s="5"/>
+      <c r="IDR5" s="5"/>
+      <c r="IEH5" s="5"/>
+      <c r="IEX5" s="5"/>
+      <c r="IFN5" s="5"/>
+      <c r="IGD5" s="5"/>
+      <c r="IGT5" s="5"/>
+      <c r="IHJ5" s="5"/>
+      <c r="IHZ5" s="5"/>
+      <c r="IIP5" s="5"/>
+      <c r="IJF5" s="5"/>
+      <c r="IJV5" s="5"/>
+      <c r="IKL5" s="5"/>
+      <c r="ILB5" s="5"/>
+      <c r="ILR5" s="5"/>
+      <c r="IMH5" s="5"/>
+      <c r="IMX5" s="5"/>
+      <c r="INN5" s="5"/>
+      <c r="IOD5" s="5"/>
+      <c r="IOT5" s="5"/>
+      <c r="IPJ5" s="5"/>
+      <c r="IPZ5" s="5"/>
+      <c r="IQP5" s="5"/>
+      <c r="IRF5" s="5"/>
+      <c r="IRV5" s="5"/>
+      <c r="ISL5" s="5"/>
+      <c r="ITB5" s="5"/>
+      <c r="ITR5" s="5"/>
+      <c r="IUH5" s="5"/>
+      <c r="IUX5" s="5"/>
+      <c r="IVN5" s="5"/>
+      <c r="IWD5" s="5"/>
+      <c r="IWT5" s="5"/>
+      <c r="IXJ5" s="5"/>
+      <c r="IXZ5" s="5"/>
+      <c r="IYP5" s="5"/>
+      <c r="IZF5" s="5"/>
+      <c r="IZV5" s="5"/>
+      <c r="JAL5" s="5"/>
+      <c r="JBB5" s="5"/>
+      <c r="JBR5" s="5"/>
+      <c r="JCH5" s="5"/>
+      <c r="JCX5" s="5"/>
+      <c r="JDN5" s="5"/>
+      <c r="JED5" s="5"/>
+      <c r="JET5" s="5"/>
+      <c r="JFJ5" s="5"/>
+      <c r="JFZ5" s="5"/>
+      <c r="JGP5" s="5"/>
+      <c r="JHF5" s="5"/>
+      <c r="JHV5" s="5"/>
+      <c r="JIL5" s="5"/>
+      <c r="JJB5" s="5"/>
+      <c r="JJR5" s="5"/>
+      <c r="JKH5" s="5"/>
+      <c r="JKX5" s="5"/>
+      <c r="JLN5" s="5"/>
+      <c r="JMD5" s="5"/>
+      <c r="JMT5" s="5"/>
+      <c r="JNJ5" s="5"/>
+      <c r="JNZ5" s="5"/>
+      <c r="JOP5" s="5"/>
+      <c r="JPF5" s="5"/>
+      <c r="JPV5" s="5"/>
+      <c r="JQL5" s="5"/>
+      <c r="JRB5" s="5"/>
+      <c r="JRR5" s="5"/>
+      <c r="JSH5" s="5"/>
+      <c r="JSX5" s="5"/>
+      <c r="JTN5" s="5"/>
+      <c r="JUD5" s="5"/>
+      <c r="JUT5" s="5"/>
+      <c r="JVJ5" s="5"/>
+      <c r="JVZ5" s="5"/>
+      <c r="JWP5" s="5"/>
+      <c r="JXF5" s="5"/>
+      <c r="JXV5" s="5"/>
+      <c r="JYL5" s="5"/>
+      <c r="JZB5" s="5"/>
+      <c r="JZR5" s="5"/>
+      <c r="KAH5" s="5"/>
+      <c r="KAX5" s="5"/>
+      <c r="KBN5" s="5"/>
+      <c r="KCD5" s="5"/>
+      <c r="KCT5" s="5"/>
+      <c r="KDJ5" s="5"/>
+      <c r="KDZ5" s="5"/>
+      <c r="KEP5" s="5"/>
+      <c r="KFF5" s="5"/>
+      <c r="KFV5" s="5"/>
+      <c r="KGL5" s="5"/>
+      <c r="KHB5" s="5"/>
+      <c r="KHR5" s="5"/>
+      <c r="KIH5" s="5"/>
+      <c r="KIX5" s="5"/>
+      <c r="KJN5" s="5"/>
+      <c r="KKD5" s="5"/>
+      <c r="KKT5" s="5"/>
+      <c r="KLJ5" s="5"/>
+      <c r="KLZ5" s="5"/>
+      <c r="KMP5" s="5"/>
+      <c r="KNF5" s="5"/>
+      <c r="KNV5" s="5"/>
+      <c r="KOL5" s="5"/>
+      <c r="KPB5" s="5"/>
+      <c r="KPR5" s="5"/>
+      <c r="KQH5" s="5"/>
+      <c r="KQX5" s="5"/>
+      <c r="KRN5" s="5"/>
+      <c r="KSD5" s="5"/>
+      <c r="KST5" s="5"/>
+      <c r="KTJ5" s="5"/>
+      <c r="KTZ5" s="5"/>
+      <c r="KUP5" s="5"/>
+      <c r="KVF5" s="5"/>
+      <c r="KVV5" s="5"/>
+      <c r="KWL5" s="5"/>
+      <c r="KXB5" s="5"/>
+      <c r="KXR5" s="5"/>
+      <c r="KYH5" s="5"/>
+      <c r="KYX5" s="5"/>
+      <c r="KZN5" s="5"/>
+      <c r="LAD5" s="5"/>
+      <c r="LAT5" s="5"/>
+      <c r="LBJ5" s="5"/>
+      <c r="LBZ5" s="5"/>
+      <c r="LCP5" s="5"/>
+      <c r="LDF5" s="5"/>
+      <c r="LDV5" s="5"/>
+      <c r="LEL5" s="5"/>
+      <c r="LFB5" s="5"/>
+      <c r="LFR5" s="5"/>
+      <c r="LGH5" s="5"/>
+      <c r="LGX5" s="5"/>
+      <c r="LHN5" s="5"/>
+      <c r="LID5" s="5"/>
+      <c r="LIT5" s="5"/>
+      <c r="LJJ5" s="5"/>
+      <c r="LJZ5" s="5"/>
+      <c r="LKP5" s="5"/>
+      <c r="LLF5" s="5"/>
+      <c r="LLV5" s="5"/>
+      <c r="LML5" s="5"/>
+      <c r="LNB5" s="5"/>
+      <c r="LNR5" s="5"/>
+      <c r="LOH5" s="5"/>
+      <c r="LOX5" s="5"/>
+      <c r="LPN5" s="5"/>
+      <c r="LQD5" s="5"/>
+      <c r="LQT5" s="5"/>
+      <c r="LRJ5" s="5"/>
+      <c r="LRZ5" s="5"/>
+      <c r="LSP5" s="5"/>
+      <c r="LTF5" s="5"/>
+      <c r="LTV5" s="5"/>
+      <c r="LUL5" s="5"/>
+      <c r="LVB5" s="5"/>
+      <c r="LVR5" s="5"/>
+      <c r="LWH5" s="5"/>
+      <c r="LWX5" s="5"/>
+      <c r="LXN5" s="5"/>
+      <c r="LYD5" s="5"/>
+      <c r="LYT5" s="5"/>
+      <c r="LZJ5" s="5"/>
+      <c r="LZZ5" s="5"/>
+      <c r="MAP5" s="5"/>
+      <c r="MBF5" s="5"/>
+      <c r="MBV5" s="5"/>
+      <c r="MCL5" s="5"/>
+      <c r="MDB5" s="5"/>
+      <c r="MDR5" s="5"/>
+      <c r="MEH5" s="5"/>
+      <c r="MEX5" s="5"/>
+      <c r="MFN5" s="5"/>
+      <c r="MGD5" s="5"/>
+      <c r="MGT5" s="5"/>
+      <c r="MHJ5" s="5"/>
+      <c r="MHZ5" s="5"/>
+      <c r="MIP5" s="5"/>
+      <c r="MJF5" s="5"/>
+      <c r="MJV5" s="5"/>
+      <c r="MKL5" s="5"/>
+      <c r="MLB5" s="5"/>
+      <c r="MLR5" s="5"/>
+      <c r="MMH5" s="5"/>
+      <c r="MMX5" s="5"/>
+      <c r="MNN5" s="5"/>
+      <c r="MOD5" s="5"/>
+      <c r="MOT5" s="5"/>
+      <c r="MPJ5" s="5"/>
+      <c r="MPZ5" s="5"/>
+      <c r="MQP5" s="5"/>
+      <c r="MRF5" s="5"/>
+      <c r="MRV5" s="5"/>
+      <c r="MSL5" s="5"/>
+      <c r="MTB5" s="5"/>
+      <c r="MTR5" s="5"/>
+      <c r="MUH5" s="5"/>
+      <c r="MUX5" s="5"/>
+      <c r="MVN5" s="5"/>
+      <c r="MWD5" s="5"/>
+      <c r="MWT5" s="5"/>
+      <c r="MXJ5" s="5"/>
+      <c r="MXZ5" s="5"/>
+      <c r="MYP5" s="5"/>
+      <c r="MZF5" s="5"/>
+      <c r="MZV5" s="5"/>
+      <c r="NAL5" s="5"/>
+      <c r="NBB5" s="5"/>
+      <c r="NBR5" s="5"/>
+      <c r="NCH5" s="5"/>
+      <c r="NCX5" s="5"/>
+      <c r="NDN5" s="5"/>
+      <c r="NED5" s="5"/>
+      <c r="NET5" s="5"/>
+      <c r="NFJ5" s="5"/>
+      <c r="NFZ5" s="5"/>
+      <c r="NGP5" s="5"/>
+      <c r="NHF5" s="5"/>
+      <c r="NHV5" s="5"/>
+      <c r="NIL5" s="5"/>
+      <c r="NJB5" s="5"/>
+      <c r="NJR5" s="5"/>
+      <c r="NKH5" s="5"/>
+      <c r="NKX5" s="5"/>
+      <c r="NLN5" s="5"/>
+      <c r="NMD5" s="5"/>
+      <c r="NMT5" s="5"/>
+      <c r="NNJ5" s="5"/>
+      <c r="NNZ5" s="5"/>
+      <c r="NOP5" s="5"/>
+      <c r="NPF5" s="5"/>
+      <c r="NPV5" s="5"/>
+      <c r="NQL5" s="5"/>
+      <c r="NRB5" s="5"/>
+      <c r="NRR5" s="5"/>
+      <c r="NSH5" s="5"/>
+      <c r="NSX5" s="5"/>
+      <c r="NTN5" s="5"/>
+      <c r="NUD5" s="5"/>
+      <c r="NUT5" s="5"/>
+      <c r="NVJ5" s="5"/>
+      <c r="NVZ5" s="5"/>
+      <c r="NWP5" s="5"/>
+      <c r="NXF5" s="5"/>
+      <c r="NXV5" s="5"/>
+      <c r="NYL5" s="5"/>
+      <c r="NZB5" s="5"/>
+      <c r="NZR5" s="5"/>
+      <c r="OAH5" s="5"/>
+      <c r="OAX5" s="5"/>
+      <c r="OBN5" s="5"/>
+      <c r="OCD5" s="5"/>
+      <c r="OCT5" s="5"/>
+      <c r="ODJ5" s="5"/>
+      <c r="ODZ5" s="5"/>
+      <c r="OEP5" s="5"/>
+      <c r="OFF5" s="5"/>
+      <c r="OFV5" s="5"/>
+      <c r="OGL5" s="5"/>
+      <c r="OHB5" s="5"/>
+      <c r="OHR5" s="5"/>
+      <c r="OIH5" s="5"/>
+      <c r="OIX5" s="5"/>
+      <c r="OJN5" s="5"/>
+      <c r="OKD5" s="5"/>
+      <c r="OKT5" s="5"/>
+      <c r="OLJ5" s="5"/>
+      <c r="OLZ5" s="5"/>
+      <c r="OMP5" s="5"/>
+      <c r="ONF5" s="5"/>
+      <c r="ONV5" s="5"/>
+      <c r="OOL5" s="5"/>
+      <c r="OPB5" s="5"/>
+      <c r="OPR5" s="5"/>
+      <c r="OQH5" s="5"/>
+      <c r="OQX5" s="5"/>
+      <c r="ORN5" s="5"/>
+      <c r="OSD5" s="5"/>
+      <c r="OST5" s="5"/>
+      <c r="OTJ5" s="5"/>
+      <c r="OTZ5" s="5"/>
+      <c r="OUP5" s="5"/>
+      <c r="OVF5" s="5"/>
+      <c r="OVV5" s="5"/>
+      <c r="OWL5" s="5"/>
+      <c r="OXB5" s="5"/>
+      <c r="OXR5" s="5"/>
+      <c r="OYH5" s="5"/>
+      <c r="OYX5" s="5"/>
+      <c r="OZN5" s="5"/>
+      <c r="PAD5" s="5"/>
+      <c r="PAT5" s="5"/>
+      <c r="PBJ5" s="5"/>
+      <c r="PBZ5" s="5"/>
+      <c r="PCP5" s="5"/>
+      <c r="PDF5" s="5"/>
+      <c r="PDV5" s="5"/>
+      <c r="PEL5" s="5"/>
+      <c r="PFB5" s="5"/>
+      <c r="PFR5" s="5"/>
+      <c r="PGH5" s="5"/>
+      <c r="PGX5" s="5"/>
+      <c r="PHN5" s="5"/>
+      <c r="PID5" s="5"/>
+      <c r="PIT5" s="5"/>
+      <c r="PJJ5" s="5"/>
+      <c r="PJZ5" s="5"/>
+      <c r="PKP5" s="5"/>
+      <c r="PLF5" s="5"/>
+      <c r="PLV5" s="5"/>
+      <c r="PML5" s="5"/>
+      <c r="PNB5" s="5"/>
+      <c r="PNR5" s="5"/>
+      <c r="POH5" s="5"/>
+      <c r="POX5" s="5"/>
+      <c r="PPN5" s="5"/>
+      <c r="PQD5" s="5"/>
+      <c r="PQT5" s="5"/>
+      <c r="PRJ5" s="5"/>
+      <c r="PRZ5" s="5"/>
+      <c r="PSP5" s="5"/>
+      <c r="PTF5" s="5"/>
+      <c r="PTV5" s="5"/>
+      <c r="PUL5" s="5"/>
+      <c r="PVB5" s="5"/>
+      <c r="PVR5" s="5"/>
+      <c r="PWH5" s="5"/>
+      <c r="PWX5" s="5"/>
+      <c r="PXN5" s="5"/>
+      <c r="PYD5" s="5"/>
+      <c r="PYT5" s="5"/>
+      <c r="PZJ5" s="5"/>
+      <c r="PZZ5" s="5"/>
+      <c r="QAP5" s="5"/>
+      <c r="QBF5" s="5"/>
+      <c r="QBV5" s="5"/>
+      <c r="QCL5" s="5"/>
+      <c r="QDB5" s="5"/>
+      <c r="QDR5" s="5"/>
+      <c r="QEH5" s="5"/>
+      <c r="QEX5" s="5"/>
+      <c r="QFN5" s="5"/>
+      <c r="QGD5" s="5"/>
+      <c r="QGT5" s="5"/>
+      <c r="QHJ5" s="5"/>
+      <c r="QHZ5" s="5"/>
+      <c r="QIP5" s="5"/>
+      <c r="QJF5" s="5"/>
+      <c r="QJV5" s="5"/>
+      <c r="QKL5" s="5"/>
+      <c r="QLB5" s="5"/>
+      <c r="QLR5" s="5"/>
+      <c r="QMH5" s="5"/>
+      <c r="QMX5" s="5"/>
+      <c r="QNN5" s="5"/>
+      <c r="QOD5" s="5"/>
+      <c r="QOT5" s="5"/>
+      <c r="QPJ5" s="5"/>
+      <c r="QPZ5" s="5"/>
+      <c r="QQP5" s="5"/>
+      <c r="QRF5" s="5"/>
+      <c r="QRV5" s="5"/>
+      <c r="QSL5" s="5"/>
+      <c r="QTB5" s="5"/>
+      <c r="QTR5" s="5"/>
+      <c r="QUH5" s="5"/>
+      <c r="QUX5" s="5"/>
+      <c r="QVN5" s="5"/>
+      <c r="QWD5" s="5"/>
+      <c r="QWT5" s="5"/>
+      <c r="QXJ5" s="5"/>
+      <c r="QXZ5" s="5"/>
+      <c r="QYP5" s="5"/>
+      <c r="QZF5" s="5"/>
+      <c r="QZV5" s="5"/>
+      <c r="RAL5" s="5"/>
+      <c r="RBB5" s="5"/>
+      <c r="RBR5" s="5"/>
+      <c r="RCH5" s="5"/>
+      <c r="RCX5" s="5"/>
+      <c r="RDN5" s="5"/>
+      <c r="RED5" s="5"/>
+      <c r="RET5" s="5"/>
+      <c r="RFJ5" s="5"/>
+      <c r="RFZ5" s="5"/>
+      <c r="RGP5" s="5"/>
+      <c r="RHF5" s="5"/>
+      <c r="RHV5" s="5"/>
+      <c r="RIL5" s="5"/>
+      <c r="RJB5" s="5"/>
+      <c r="RJR5" s="5"/>
+      <c r="RKH5" s="5"/>
+      <c r="RKX5" s="5"/>
+      <c r="RLN5" s="5"/>
+      <c r="RMD5" s="5"/>
+      <c r="RMT5" s="5"/>
+      <c r="RNJ5" s="5"/>
+      <c r="RNZ5" s="5"/>
+      <c r="ROP5" s="5"/>
+      <c r="RPF5" s="5"/>
+      <c r="RPV5" s="5"/>
+      <c r="RQL5" s="5"/>
+      <c r="RRB5" s="5"/>
+      <c r="RRR5" s="5"/>
+      <c r="RSH5" s="5"/>
+      <c r="RSX5" s="5"/>
+      <c r="RTN5" s="5"/>
+      <c r="RUD5" s="5"/>
+      <c r="RUT5" s="5"/>
+      <c r="RVJ5" s="5"/>
+      <c r="RVZ5" s="5"/>
+      <c r="RWP5" s="5"/>
+      <c r="RXF5" s="5"/>
+      <c r="RXV5" s="5"/>
+      <c r="RYL5" s="5"/>
+      <c r="RZB5" s="5"/>
+      <c r="RZR5" s="5"/>
+      <c r="SAH5" s="5"/>
+      <c r="SAX5" s="5"/>
+      <c r="SBN5" s="5"/>
+      <c r="SCD5" s="5"/>
+      <c r="SCT5" s="5"/>
+      <c r="SDJ5" s="5"/>
+      <c r="SDZ5" s="5"/>
+      <c r="SEP5" s="5"/>
+      <c r="SFF5" s="5"/>
+      <c r="SFV5" s="5"/>
+      <c r="SGL5" s="5"/>
+      <c r="SHB5" s="5"/>
+      <c r="SHR5" s="5"/>
+      <c r="SIH5" s="5"/>
+      <c r="SIX5" s="5"/>
+      <c r="SJN5" s="5"/>
+      <c r="SKD5" s="5"/>
+      <c r="SKT5" s="5"/>
+      <c r="SLJ5" s="5"/>
+      <c r="SLZ5" s="5"/>
+      <c r="SMP5" s="5"/>
+      <c r="SNF5" s="5"/>
+      <c r="SNV5" s="5"/>
+      <c r="SOL5" s="5"/>
+      <c r="SPB5" s="5"/>
+      <c r="SPR5" s="5"/>
+      <c r="SQH5" s="5"/>
+      <c r="SQX5" s="5"/>
+      <c r="SRN5" s="5"/>
+      <c r="SSD5" s="5"/>
+      <c r="SST5" s="5"/>
+      <c r="STJ5" s="5"/>
+      <c r="STZ5" s="5"/>
+      <c r="SUP5" s="5"/>
+      <c r="SVF5" s="5"/>
+      <c r="SVV5" s="5"/>
+      <c r="SWL5" s="5"/>
+      <c r="SXB5" s="5"/>
+      <c r="SXR5" s="5"/>
+      <c r="SYH5" s="5"/>
+      <c r="SYX5" s="5"/>
+      <c r="SZN5" s="5"/>
+      <c r="TAD5" s="5"/>
+      <c r="TAT5" s="5"/>
+      <c r="TBJ5" s="5"/>
+      <c r="TBZ5" s="5"/>
+      <c r="TCP5" s="5"/>
+      <c r="TDF5" s="5"/>
+      <c r="TDV5" s="5"/>
+      <c r="TEL5" s="5"/>
+      <c r="TFB5" s="5"/>
+      <c r="TFR5" s="5"/>
+      <c r="TGH5" s="5"/>
+      <c r="TGX5" s="5"/>
+      <c r="THN5" s="5"/>
+      <c r="TID5" s="5"/>
+      <c r="TIT5" s="5"/>
+      <c r="TJJ5" s="5"/>
+      <c r="TJZ5" s="5"/>
+      <c r="TKP5" s="5"/>
+      <c r="TLF5" s="5"/>
+      <c r="TLV5" s="5"/>
+      <c r="TML5" s="5"/>
+      <c r="TNB5" s="5"/>
+      <c r="TNR5" s="5"/>
+      <c r="TOH5" s="5"/>
+      <c r="TOX5" s="5"/>
+      <c r="TPN5" s="5"/>
+      <c r="TQD5" s="5"/>
+      <c r="TQT5" s="5"/>
+      <c r="TRJ5" s="5"/>
+      <c r="TRZ5" s="5"/>
+      <c r="TSP5" s="5"/>
+      <c r="TTF5" s="5"/>
+      <c r="TTV5" s="5"/>
+      <c r="TUL5" s="5"/>
+      <c r="TVB5" s="5"/>
+      <c r="TVR5" s="5"/>
+      <c r="TWH5" s="5"/>
+      <c r="TWX5" s="5"/>
+      <c r="TXN5" s="5"/>
+      <c r="TYD5" s="5"/>
+      <c r="TYT5" s="5"/>
+      <c r="TZJ5" s="5"/>
+      <c r="TZZ5" s="5"/>
+      <c r="UAP5" s="5"/>
+      <c r="UBF5" s="5"/>
+      <c r="UBV5" s="5"/>
+      <c r="UCL5" s="5"/>
+      <c r="UDB5" s="5"/>
+      <c r="UDR5" s="5"/>
+      <c r="UEH5" s="5"/>
+      <c r="UEX5" s="5"/>
+      <c r="UFN5" s="5"/>
+      <c r="UGD5" s="5"/>
+      <c r="UGT5" s="5"/>
+      <c r="UHJ5" s="5"/>
+      <c r="UHZ5" s="5"/>
+      <c r="UIP5" s="5"/>
+      <c r="UJF5" s="5"/>
+      <c r="UJV5" s="5"/>
+      <c r="UKL5" s="5"/>
+      <c r="ULB5" s="5"/>
+      <c r="ULR5" s="5"/>
+      <c r="UMH5" s="5"/>
+      <c r="UMX5" s="5"/>
+      <c r="UNN5" s="5"/>
+      <c r="UOD5" s="5"/>
+      <c r="UOT5" s="5"/>
+      <c r="UPJ5" s="5"/>
+      <c r="UPZ5" s="5"/>
+      <c r="UQP5" s="5"/>
+      <c r="URF5" s="5"/>
+      <c r="URV5" s="5"/>
+      <c r="USL5" s="5"/>
+      <c r="UTB5" s="5"/>
+      <c r="UTR5" s="5"/>
+      <c r="UUH5" s="5"/>
+      <c r="UUX5" s="5"/>
+      <c r="UVN5" s="5"/>
+      <c r="UWD5" s="5"/>
+      <c r="UWT5" s="5"/>
+      <c r="UXJ5" s="5"/>
+      <c r="UXZ5" s="5"/>
+      <c r="UYP5" s="5"/>
+      <c r="UZF5" s="5"/>
+      <c r="UZV5" s="5"/>
+      <c r="VAL5" s="5"/>
+      <c r="VBB5" s="5"/>
+      <c r="VBR5" s="5"/>
+      <c r="VCH5" s="5"/>
+      <c r="VCX5" s="5"/>
+      <c r="VDN5" s="5"/>
+      <c r="VED5" s="5"/>
+      <c r="VET5" s="5"/>
+      <c r="VFJ5" s="5"/>
+      <c r="VFZ5" s="5"/>
+      <c r="VGP5" s="5"/>
+      <c r="VHF5" s="5"/>
+      <c r="VHV5" s="5"/>
+      <c r="VIL5" s="5"/>
+      <c r="VJB5" s="5"/>
+      <c r="VJR5" s="5"/>
+      <c r="VKH5" s="5"/>
+      <c r="VKX5" s="5"/>
+      <c r="VLN5" s="5"/>
+      <c r="VMD5" s="5"/>
+      <c r="VMT5" s="5"/>
+      <c r="VNJ5" s="5"/>
+      <c r="VNZ5" s="5"/>
+      <c r="VOP5" s="5"/>
+      <c r="VPF5" s="5"/>
+      <c r="VPV5" s="5"/>
+      <c r="VQL5" s="5"/>
+      <c r="VRB5" s="5"/>
+      <c r="VRR5" s="5"/>
+      <c r="VSH5" s="5"/>
+      <c r="VSX5" s="5"/>
+      <c r="VTN5" s="5"/>
+      <c r="VUD5" s="5"/>
+      <c r="VUT5" s="5"/>
+      <c r="VVJ5" s="5"/>
+      <c r="VVZ5" s="5"/>
+      <c r="VWP5" s="5"/>
+      <c r="VXF5" s="5"/>
+      <c r="VXV5" s="5"/>
+      <c r="VYL5" s="5"/>
+      <c r="VZB5" s="5"/>
+      <c r="VZR5" s="5"/>
+      <c r="WAH5" s="5"/>
+      <c r="WAX5" s="5"/>
+      <c r="WBN5" s="5"/>
+      <c r="WCD5" s="5"/>
+      <c r="WCT5" s="5"/>
+      <c r="WDJ5" s="5"/>
+      <c r="WDZ5" s="5"/>
+      <c r="WEP5" s="5"/>
+      <c r="WFF5" s="5"/>
+      <c r="WFV5" s="5"/>
+      <c r="WGL5" s="5"/>
+      <c r="WHB5" s="5"/>
+      <c r="WHR5" s="5"/>
+      <c r="WIH5" s="5"/>
+      <c r="WIX5" s="5"/>
+      <c r="WJN5" s="5"/>
+      <c r="WKD5" s="5"/>
+      <c r="WKT5" s="5"/>
+      <c r="WLJ5" s="5"/>
+      <c r="WLZ5" s="5"/>
+      <c r="WMP5" s="5"/>
+      <c r="WNF5" s="5"/>
+      <c r="WNV5" s="5"/>
+      <c r="WOL5" s="5"/>
+      <c r="WPB5" s="5"/>
+      <c r="WPR5" s="5"/>
+      <c r="WQH5" s="5"/>
+      <c r="WQX5" s="5"/>
+      <c r="WRN5" s="5"/>
+      <c r="WSD5" s="5"/>
+      <c r="WST5" s="5"/>
+      <c r="WTJ5" s="5"/>
+      <c r="WTZ5" s="5"/>
+      <c r="WUP5" s="5"/>
+      <c r="WVF5" s="5"/>
+      <c r="WVV5" s="5"/>
+      <c r="WWL5" s="5"/>
+      <c r="WXB5" s="5"/>
+      <c r="WXR5" s="5"/>
+      <c r="WYH5" s="5"/>
+      <c r="WYX5" s="5"/>
+      <c r="WZN5" s="5"/>
+      <c r="XAD5" s="5"/>
+      <c r="XAT5" s="5"/>
+      <c r="XBJ5" s="5"/>
+      <c r="XBZ5" s="5"/>
+      <c r="XCP5" s="5"/>
+      <c r="XDF5" s="5"/>
+      <c r="XDV5" s="5"/>
+      <c r="XEL5" s="5"/>
+      <c r="XFB5" s="5"/>
+    </row>
+    <row r="6" spans="1:1022 1038:2046 2062:3070 3086:4094 4110:5118 5134:6142 6158:7166 7182:8190 8206:9214 9230:10238 10254:11262 11278:12286 12302:13310 13326:14334 14350:15358 15374:16382" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="I5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="F6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" t="s">
-        <v>10</v>
+      <c r="G6" t="s">
+        <v>60</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="K6">
+        <v>200</v>
       </c>
       <c r="L6" t="s">
-        <v>11</v>
+        <v>60</v>
+      </c>
+      <c r="N6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1022 1038:2046 2062:3070 3086:4094 4110:5118 5134:6142 6158:7166 7182:8190 8206:9214 9230:10238 10254:11262 11278:12286 12302:13310 13326:14334 14350:15358 15374:16382" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>400</v>
+      </c>
+      <c r="L7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" t="s">
+        <v>62</v>
+      </c>
+      <c r="P7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1022 1038:2046 2062:3070 3086:4094 4110:5118 5134:6142 6158:7166 7182:8190 8206:9214 9230:10238 10254:11262 11278:12286 12302:13310 13326:14334 14350:15358 15374:16382" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>66</v>
+      </c>
+      <c r="O8" t="s">
+        <v>65</v>
+      </c>
+      <c r="P8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1022 1038:2046 2062:3070 3086:4094 4110:5118 5134:6142 6158:7166 7182:8190 8206:9214 9230:10238 10254:11262 11278:12286 12302:13310 13326:14334 14350:15358 15374:16382" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>200</v>
+      </c>
+      <c r="L9" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -736,9 +1880,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,15 +1909,15 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -782,251 +1926,251 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J5" t="s">
         <v>4</v>
       </c>
       <c r="K5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="L5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="M5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="O5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="P5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>10</v>
+      <c r="A6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="J6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K6">
         <v>200</v>
       </c>
       <c r="L6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="7"/>
-      <c r="F7" s="6"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="10"/>
+      <c r="F7" s="15"/>
       <c r="K7">
         <v>500</v>
       </c>
       <c r="L7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>10</v>
+      <c r="J8" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="K8" s="3">
         <v>200</v>
       </c>
       <c r="L8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="O8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="P8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
       <c r="K9">
         <v>500</v>
       </c>
       <c r="L9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="O9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="P9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
       <c r="K10">
         <v>400</v>
       </c>
       <c r="L10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="O10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="P10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
       <c r="K11">
         <v>500</v>
       </c>
       <c r="L11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="O11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="P11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
       <c r="K12">
         <v>400</v>
       </c>
       <c r="L12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="O12" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="P12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>61</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="I13" t="s">
-        <v>56</v>
-      </c>
-      <c r="J13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="D14" s="2"/>
       <c r="F14" s="2"/>
@@ -1034,16 +2178,16 @@
         <v>500</v>
       </c>
       <c r="L14" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="O14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="D15" s="2"/>
       <c r="F15" s="2"/>
@@ -1051,10 +2195,10 @@
         <v>200</v>
       </c>
       <c r="L15" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1249,21 +2393,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
     <mergeCell ref="F8:F12"/>
     <mergeCell ref="G8:G12"/>
     <mergeCell ref="H8:H12"/>
     <mergeCell ref="I8:I12"/>
     <mergeCell ref="J8:J12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="E8:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
ITO-000 Create endpoint contest-005, 006
</commit_message>
<xml_diff>
--- a/document/contest-endpoint.xlsx
+++ b/document/contest-endpoint.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="3465" tabRatio="576" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="3465" tabRatio="576" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="2" r:id="rId1"/>
     <sheet name="contests" sheetId="3" r:id="rId2"/>
     <sheet name="problem" sheetId="1" r:id="rId3"/>
+    <sheet name="judgehost" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="100">
   <si>
     <t>Context path</t>
   </si>
@@ -234,24 +235,15 @@
     <t>Get all Contest belong to currect user login (admin of contest)</t>
   </si>
   <si>
-    <t>/contest</t>
-  </si>
-  <si>
     <t>List&lt;onlinejudge.domain.Contest&gt;</t>
   </si>
   <si>
     <t>#contest-003</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>#contest-004</t>
   </si>
   <si>
-    <t>/contest/{contestID}/problems</t>
-  </si>
-  <si>
     <t>problem-request-002.json</t>
   </si>
   <si>
@@ -273,13 +265,69 @@
     <t>Add Team to Contest. New Team will be appended in to List Team</t>
   </si>
   <si>
-    <t>/contest/{contestID}/addteam</t>
-  </si>
-  <si>
     <t>contest-request-004.json</t>
   </si>
   <si>
     <t>onlinejudge.domain.Team</t>
+  </si>
+  <si>
+    <t>#judgehost-001</t>
+  </si>
+  <si>
+    <t>Submit Java file to judge</t>
+  </si>
+  <si>
+    <t>/judgehost</t>
+  </si>
+  <si>
+    <t>teamId: string
+problemId: string
+file: binary</t>
+  </si>
+  <si>
+    <t>Accepted: correct answer
+WrongAnswer: Wrong Answer
+CompileFail: Compile Fail</t>
+  </si>
+  <si>
+    <t>#contest-005</t>
+  </si>
+  <si>
+    <t>onlinejudge.domain.Submit</t>
+  </si>
+  <si>
+    <t>Create Submit success</t>
+  </si>
+  <si>
+    <t>#contest=006</t>
+  </si>
+  <si>
+    <t>Add or update Submit of team. MS Judge use.</t>
+  </si>
+  <si>
+    <t>Get Problem by ProblemForContest's id.</t>
+  </si>
+  <si>
+    <t>/contests/{contestID}/problems</t>
+  </si>
+  <si>
+    <t>/contests/{contestID}/addteam</t>
+  </si>
+  <si>
+    <t>/contests/team/submit</t>
+  </si>
+  <si>
+    <t>/contests/problem_for_contest/problem</t>
+  </si>
+  <si>
+    <t>problemForContestId</t>
+  </si>
+  <si>
+    <t>idTeam: string
+idContest: string
+idProblemForTeam: string
+file: binary
+isOverrideTestCase: boolean</t>
   </si>
 </sst>
 </file>
@@ -309,7 +357,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -317,11 +365,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -333,15 +396,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -360,9 +417,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -370,7 +424,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -379,10 +445,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -729,22 +798,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:Q13"/>
+  <dimension ref="A3:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
     <col min="6" max="6" width="23.5703125" customWidth="1"/>
     <col min="7" max="8" width="28.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.5703125" customWidth="1"/>
     <col min="11" max="11" width="23.28515625" customWidth="1"/>
     <col min="12" max="12" width="35.42578125" customWidth="1"/>
@@ -803,7 +872,7 @@
       <c r="M5" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="O5" t="s">
@@ -814,7 +883,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="10" t="s">
         <v>58</v>
       </c>
       <c r="B6" t="s">
@@ -833,7 +902,7 @@
         <v>60</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J6" t="s">
         <v>8</v>
@@ -877,14 +946,14 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
         <v>50</v>
@@ -902,50 +971,47 @@
         <v>200</v>
       </c>
       <c r="L9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>82</v>
+      <c r="B11" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
-      <c r="E11" t="s">
-        <v>74</v>
-      </c>
       <c r="G11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K11">
         <v>200</v>
       </c>
       <c r="L11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Q11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>84</v>
+      <c r="C13" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -954,10 +1020,10 @@
         <v>8</v>
       </c>
       <c r="G13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H13" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J13" t="s">
         <v>8</v>
@@ -966,10 +1032,71 @@
         <v>200</v>
       </c>
       <c r="L13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="Q13" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K15">
+        <v>200</v>
+      </c>
+      <c r="L15" t="s">
+        <v>89</v>
+      </c>
+      <c r="N15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" t="s">
+        <v>98</v>
+      </c>
+      <c r="J17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17">
+        <v>200</v>
+      </c>
+      <c r="L17" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -983,7 +1110,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H8" sqref="H8:H12"/>
+      <selection pane="topRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,7 +1127,7 @@
     <col min="10" max="11" width="14.5703125" customWidth="1"/>
     <col min="12" max="12" width="32.140625" customWidth="1"/>
     <col min="13" max="13" width="23.28515625" customWidth="1"/>
-    <col min="14" max="14" width="26.140625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="26.140625" style="4" customWidth="1"/>
     <col min="15" max="15" width="27.85546875" customWidth="1"/>
     <col min="16" max="16" width="47.5703125" customWidth="1"/>
   </cols>
@@ -1053,7 +1180,7 @@
       <c r="M5" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="O5" t="s">
@@ -1064,19 +1191,19 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="19" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="20" t="s">
         <v>8</v>
       </c>
       <c r="G6" t="s">
@@ -1094,48 +1221,48 @@
       <c r="L6" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="18"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="16"/>
-      <c r="F7" s="19"/>
+      <c r="F7" s="20"/>
       <c r="K7">
         <v>500</v>
       </c>
       <c r="L7" t="s">
         <v>22</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="21" t="s">
         <v>31</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="20"/>
+      <c r="G8" s="17"/>
       <c r="H8" s="16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I8" s="16" t="s">
         <v>33</v>
@@ -1157,13 +1284,13 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="16"/>
-      <c r="G9" s="20"/>
+      <c r="G9" s="17"/>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
@@ -1181,13 +1308,13 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="16"/>
-      <c r="G10" s="20"/>
+      <c r="G10" s="17"/>
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
@@ -1205,13 +1332,13 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="16"/>
-      <c r="G11" s="20"/>
+      <c r="G11" s="17"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
@@ -1229,13 +1356,13 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="16"/>
-      <c r="E12" s="17"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="16"/>
-      <c r="G12" s="20"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
@@ -1253,23 +1380,26 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="E13" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="F13" s="2"/>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1300,7 +1430,7 @@
       <c r="L15" t="s">
         <v>55</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1496,23 +1626,140 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
     <mergeCell ref="F8:F12"/>
     <mergeCell ref="G8:G12"/>
     <mergeCell ref="H8:H12"/>
     <mergeCell ref="I8:I12"/>
     <mergeCell ref="J8:J12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="E8:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:P4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.28515625" customWidth="1"/>
+    <col min="13" max="13" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <v>200</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ITO-000 Update API create Problem
</commit_message>
<xml_diff>
--- a/document/contest-endpoint.xlsx
+++ b/document/contest-endpoint.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="3465" tabRatio="576" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="3465" tabRatio="576" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="2" r:id="rId1"/>
     <sheet name="contests" sheetId="3" r:id="rId2"/>
     <sheet name="problem" sheetId="1" r:id="rId3"/>
     <sheet name="judgehost" sheetId="4" r:id="rId4"/>
+    <sheet name="state" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="170">
   <si>
     <t>Context path</t>
   </si>
@@ -95,9 +96,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>Create new Problem without test case</t>
   </si>
   <si>
     <t>problem-request-001.json</t>
@@ -328,6 +326,219 @@
 idProblemForTeam: string
 file: binary
 isOverrideTestCase: boolean</t>
+  </si>
+  <si>
+    <t>Show detail of Submit</t>
+  </si>
+  <si>
+    <t>/contests/[contestId]/problem/[problemId]/submits/[submitId]</t>
+  </si>
+  <si>
+    <t>/[submitId]</t>
+  </si>
+  <si>
+    <t>detail</t>
+  </si>
+  <si>
+    <t>submits</t>
+  </si>
+  <si>
+    <t>problem</t>
+  </si>
+  <si>
+    <t>contests.detail</t>
+  </si>
+  <si>
+    <t>Show all Submits of a Problem of a Contest</t>
+  </si>
+  <si>
+    <t>/contests/[contestId]/problem/[problemId]/submits</t>
+  </si>
+  <si>
+    <t>/submits</t>
+  </si>
+  <si>
+    <t>Show a specific Problem of Contest</t>
+  </si>
+  <si>
+    <t>/contests/[contestId]/problem/[problemId]</t>
+  </si>
+  <si>
+    <t>/problem/[problemId]</t>
+  </si>
+  <si>
+    <t>Show all Problem of Contest</t>
+  </si>
+  <si>
+    <t>/contests/[contestId]/problems</t>
+  </si>
+  <si>
+    <t>problems</t>
+  </si>
+  <si>
+    <t>Show Scoreboard of exist Contest</t>
+  </si>
+  <si>
+    <t>/contests/[contestId]/scoreboard</t>
+  </si>
+  <si>
+    <t>/scoreboard</t>
+  </si>
+  <si>
+    <t>scoreboard</t>
+  </si>
+  <si>
+    <t>Show Contest detail</t>
+  </si>
+  <si>
+    <t>/contests/[contestId]</t>
+  </si>
+  <si>
+    <t>Show all Contest available for user</t>
+  </si>
+  <si>
+    <t>contests</t>
+  </si>
+  <si>
+    <t>Admin add new Team to exist Contest</t>
+  </si>
+  <si>
+    <t>/contest/[contestId]/team</t>
+  </si>
+  <si>
+    <t>/[contestId]/team</t>
+  </si>
+  <si>
+    <t>contest.team</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Admin update problems for exist Contest</t>
+  </si>
+  <si>
+    <t>/contest/[contestId]/problem</t>
+  </si>
+  <si>
+    <t>/[contestId]/problem</t>
+  </si>
+  <si>
+    <t>contest.problems</t>
+  </si>
+  <si>
+    <t>Admin edit exist Contest</t>
+  </si>
+  <si>
+    <t>/contest/[contestId]/edit</t>
+  </si>
+  <si>
+    <t>/[contestId]/edit</t>
+  </si>
+  <si>
+    <t>contest.edit</t>
+  </si>
+  <si>
+    <t>Admin review exist Contest</t>
+  </si>
+  <si>
+    <t>/contest/[contestId]</t>
+  </si>
+  <si>
+    <t>/[contestId]</t>
+  </si>
+  <si>
+    <t>contest.show</t>
+  </si>
+  <si>
+    <t>Admin add new Contest</t>
+  </si>
+  <si>
+    <t>/contest/add</t>
+  </si>
+  <si>
+    <t>/add</t>
+  </si>
+  <si>
+    <t>contest.add</t>
+  </si>
+  <si>
+    <t>(Show control to manage the contest)</t>
+  </si>
+  <si>
+    <t>/contest</t>
+  </si>
+  <si>
+    <t>contest</t>
+  </si>
+  <si>
+    <t>Add or update new TestCase for Problem</t>
+  </si>
+  <si>
+    <t>/problems/[problemId]/addtestcase</t>
+  </si>
+  <si>
+    <t>problem.detail.testcase</t>
+  </si>
+  <si>
+    <t>Show detail of Problem</t>
+  </si>
+  <si>
+    <t>/problems/[problemId]</t>
+  </si>
+  <si>
+    <t>/promblem/[problemId]</t>
+  </si>
+  <si>
+    <t>problem.detail</t>
+  </si>
+  <si>
+    <t>Add new Problem</t>
+  </si>
+  <si>
+    <t>/problems/add</t>
+  </si>
+  <si>
+    <t>problems.add</t>
+  </si>
+  <si>
+    <t>Show all problems of current user login</t>
+  </si>
+  <si>
+    <t>Admin management page</t>
+  </si>
+  <si>
+    <t>/management</t>
+  </si>
+  <si>
+    <t>management</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>/register</t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>/login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">login </t>
+  </si>
+  <si>
+    <t>All URL</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Create new Problem. Update if Problem have ID</t>
   </si>
 </sst>
 </file>
@@ -384,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -430,6 +641,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -438,6 +661,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -446,12 +672,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -800,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:Q17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +1049,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -873,24 +1093,24 @@
         <v>13</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O5" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5" t="s">
         <v>37</v>
-      </c>
-      <c r="P5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
         <v>58</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" t="s">
-        <v>59</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -899,10 +1119,10 @@
         <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J6" t="s">
         <v>8</v>
@@ -911,10 +1131,10 @@
         <v>200</v>
       </c>
       <c r="L6" t="s">
+        <v>59</v>
+      </c>
+      <c r="N6" t="s">
         <v>60</v>
-      </c>
-      <c r="N6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -925,44 +1145,44 @@
         <v>22</v>
       </c>
       <c r="N7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O7" t="s">
+        <v>61</v>
+      </c>
+      <c r="P7" t="s">
         <v>62</v>
-      </c>
-      <c r="P7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J9" t="s">
         <v>8</v>
@@ -971,47 +1191,47 @@
         <v>200</v>
       </c>
       <c r="L9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K11">
         <v>200</v>
       </c>
       <c r="L11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q11" t="s">
         <v>76</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -1020,10 +1240,10 @@
         <v>8</v>
       </c>
       <c r="G13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J13" t="s">
         <v>8</v>
@@ -1032,21 +1252,21 @@
         <v>200</v>
       </c>
       <c r="L13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -1055,7 +1275,7 @@
         <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J15" t="s">
         <v>8</v>
@@ -1064,30 +1284,30 @@
         <v>200</v>
       </c>
       <c r="L15" t="s">
+        <v>88</v>
+      </c>
+      <c r="N15" t="s">
         <v>89</v>
-      </c>
-      <c r="N15" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
         <v>97</v>
       </c>
-      <c r="D17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" t="s">
-        <v>98</v>
-      </c>
       <c r="I17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J17" t="s">
         <v>8</v>
@@ -1108,9 +1328,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:P57"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B16" sqref="B16"/>
+      <selection pane="topRight" activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,7 +1357,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1181,36 +1401,36 @@
         <v>13</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O5" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5" t="s">
         <v>37</v>
       </c>
-      <c r="P5" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="19" t="s">
+      <c r="B6" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="25" t="s">
         <v>8</v>
       </c>
       <c r="G6" t="s">
         <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J6" t="s">
         <v>8</v>
@@ -1222,15 +1442,15 @@
         <v>21</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="16"/>
-      <c r="F7" s="20"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="20"/>
+      <c r="F7" s="25"/>
       <c r="K7">
         <v>500</v>
       </c>
@@ -1238,36 +1458,36 @@
         <v>22</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="D8" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="20" t="s">
         <v>8</v>
       </c>
       <c r="K8" s="3">
@@ -1277,23 +1497,23 @@
         <v>22</v>
       </c>
       <c r="O8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P8" t="s">
         <v>39</v>
       </c>
-      <c r="P8" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="9" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
       <c r="K9">
         <v>500</v>
       </c>
@@ -1301,23 +1521,23 @@
         <v>22</v>
       </c>
       <c r="O9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
       <c r="K10">
         <v>400</v>
       </c>
@@ -1325,23 +1545,23 @@
         <v>22</v>
       </c>
       <c r="O10" t="s">
+        <v>42</v>
+      </c>
+      <c r="P10" t="s">
         <v>43</v>
       </c>
-      <c r="P10" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
       <c r="K11">
         <v>500</v>
       </c>
@@ -1349,23 +1569,23 @@
         <v>22</v>
       </c>
       <c r="O11" t="s">
+        <v>44</v>
+      </c>
+      <c r="P11" t="s">
         <v>45</v>
       </c>
-      <c r="P11" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
       <c r="K12">
         <v>400</v>
       </c>
@@ -1373,31 +1593,31 @@
         <v>22</v>
       </c>
       <c r="O12" t="s">
+        <v>46</v>
+      </c>
+      <c r="P12" t="s">
         <v>47</v>
       </c>
-      <c r="P12" t="s">
+    </row>
+    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
-        <v>49</v>
-      </c>
       <c r="B13" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>50</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>51</v>
       </c>
       <c r="F13" s="2"/>
       <c r="I13" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>8</v>
@@ -1414,10 +1634,10 @@
         <v>22</v>
       </c>
       <c r="O14" t="s">
+        <v>51</v>
+      </c>
+      <c r="P14" t="s">
         <v>52</v>
-      </c>
-      <c r="P14" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -1428,10 +1648,10 @@
         <v>200</v>
       </c>
       <c r="L15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1651,8 +1871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,36 +1935,36 @@
         <v>13</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" t="s">
         <v>37</v>
-      </c>
-      <c r="P3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>8</v>
@@ -1756,10 +1976,398 @@
         <v>22</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:J24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="31.140625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="16" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" customWidth="1"/>
+    <col min="8" max="8" width="36.140625" customWidth="1"/>
+    <col min="9" max="9" width="60.5703125" customWidth="1"/>
+    <col min="10" max="10" width="43.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="18">
+        <v>1</v>
+      </c>
+      <c r="E4" s="16">
+        <v>2</v>
+      </c>
+      <c r="F4" s="16">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>167</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="H5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I5" t="s">
+        <v>165</v>
+      </c>
+      <c r="J5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D6" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="H6" t="s">
+        <v>162</v>
+      </c>
+      <c r="I6" t="s">
+        <v>162</v>
+      </c>
+      <c r="J6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="H7" t="s">
+        <v>159</v>
+      </c>
+      <c r="I7" t="s">
+        <v>159</v>
+      </c>
+      <c r="J7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="H9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I9" t="s">
+        <v>155</v>
+      </c>
+      <c r="J9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="H10" t="s">
+        <v>152</v>
+      </c>
+      <c r="I10" t="s">
+        <v>151</v>
+      </c>
+      <c r="J10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="H11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I11" t="s">
+        <v>148</v>
+      </c>
+      <c r="J11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="H12" t="s">
+        <v>145</v>
+      </c>
+      <c r="I12" t="s">
+        <v>145</v>
+      </c>
+      <c r="J12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="H13" t="s">
+        <v>142</v>
+      </c>
+      <c r="I13" t="s">
+        <v>141</v>
+      </c>
+      <c r="J13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="H14" t="s">
+        <v>138</v>
+      </c>
+      <c r="I14" t="s">
+        <v>137</v>
+      </c>
+      <c r="J14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="H15" t="s">
+        <v>134</v>
+      </c>
+      <c r="I15" t="s">
+        <v>133</v>
+      </c>
+      <c r="J15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="H16" t="s">
+        <v>130</v>
+      </c>
+      <c r="I16" t="s">
+        <v>129</v>
+      </c>
+      <c r="J16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="H17" t="s">
+        <v>125</v>
+      </c>
+      <c r="I17" t="s">
+        <v>124</v>
+      </c>
+      <c r="J17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D18" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="H18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D19" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="H19" t="s">
+        <v>120</v>
+      </c>
+      <c r="I19" t="s">
+        <v>120</v>
+      </c>
+      <c r="J19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D20" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H20" t="s">
+        <v>117</v>
+      </c>
+      <c r="I20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D21" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H21" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" t="s">
+        <v>113</v>
+      </c>
+      <c r="J21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D22" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="H22" t="s">
+        <v>111</v>
+      </c>
+      <c r="I22" t="s">
+        <v>110</v>
+      </c>
+      <c r="J22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D23" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="H23" t="s">
+        <v>108</v>
+      </c>
+      <c r="I23" t="s">
+        <v>107</v>
+      </c>
+      <c r="J23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D24" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" t="s">
+        <v>102</v>
+      </c>
+      <c r="H24" t="s">
+        <v>101</v>
+      </c>
+      <c r="I24" t="s">
+        <v>100</v>
+      </c>
+      <c r="J24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ITO-000 add API delete Problem
</commit_message>
<xml_diff>
--- a/document/contest-endpoint.xlsx
+++ b/document/contest-endpoint.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="176">
   <si>
     <t>Context path</t>
   </si>
@@ -540,12 +540,30 @@
   <si>
     <t>Create new Problem. Update if Problem have ID</t>
   </si>
+  <si>
+    <t>#problem-004</t>
+  </si>
+  <si>
+    <t>Delete Problem by id</t>
+  </si>
+  <si>
+    <t>/problems/delete</t>
+  </si>
+  <si>
+    <t>problemID</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>TODO: create detail desciption</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -553,8 +571,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -564,6 +589,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -595,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -652,27 +683,31 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1330,7 +1365,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B6" sqref="B6:B7"/>
+      <selection pane="topRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,16 +1446,16 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="23" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="25" t="s">
@@ -1446,10 +1481,10 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="20"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
       <c r="F7" s="25"/>
       <c r="K7">
         <v>500</v>
@@ -1462,32 +1497,32 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="20" t="s">
+      <c r="G8" s="26"/>
+      <c r="H8" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="23" t="s">
         <v>8</v>
       </c>
       <c r="K8" s="3">
@@ -1504,16 +1539,16 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
       <c r="K9">
         <v>500</v>
       </c>
@@ -1528,16 +1563,16 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
       <c r="K10">
         <v>400</v>
       </c>
@@ -1552,16 +1587,16 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
       <c r="K11">
         <v>500</v>
       </c>
@@ -1576,16 +1611,16 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
       <c r="K12">
         <v>400</v>
       </c>
@@ -1624,9 +1659,6 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="F14" s="2"/>
       <c r="K14">
         <v>500</v>
       </c>
@@ -1655,9 +1687,27 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="A16" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" t="s">
+        <v>172</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>173</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -1846,21 +1896,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="F8:F12"/>
+    <mergeCell ref="G8:G12"/>
+    <mergeCell ref="H8:H12"/>
+    <mergeCell ref="I8:I12"/>
+    <mergeCell ref="J8:J12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="B8:B12"/>
     <mergeCell ref="C8:C12"/>
     <mergeCell ref="D8:D12"/>
     <mergeCell ref="E8:E12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F8:F12"/>
-    <mergeCell ref="G8:G12"/>
-    <mergeCell ref="H8:H12"/>
-    <mergeCell ref="I8:I12"/>
-    <mergeCell ref="J8:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
ITO-000 create API delete team in input
</commit_message>
<xml_diff>
--- a/document/contest-endpoint.xlsx
+++ b/document/contest-endpoint.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="187">
   <si>
     <t>Context path</t>
   </si>
@@ -569,6 +569,27 @@
   </si>
   <si>
     <t>Delete Success</t>
+  </si>
+  <si>
+    <t>#contest-008</t>
+  </si>
+  <si>
+    <t>Get All Contest in which, current user is member of a team.</t>
+  </si>
+  <si>
+    <t>Get success</t>
+  </si>
+  <si>
+    <t>/contest/contest_as_member</t>
+  </si>
+  <si>
+    <t>#contest-009</t>
+  </si>
+  <si>
+    <t>Delete a Team of Contest.</t>
+  </si>
+  <si>
+    <t>/contest/{contestID}/delete_team/{teamID}</t>
   </si>
 </sst>
 </file>
@@ -638,7 +659,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -699,6 +720,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1065,17 +1095,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:Q19"/>
+  <dimension ref="A3:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="41" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" customWidth="1"/>
+    <col min="3" max="3" width="44.5703125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="23.28515625" customWidth="1"/>
     <col min="6" max="6" width="23.5703125" customWidth="1"/>
@@ -1305,25 +1335,24 @@
         <v>76</v>
       </c>
     </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+    </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" t="s">
-        <v>94</v>
+      <c r="A15" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>186</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
       </c>
-      <c r="F15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" t="s">
-        <v>88</v>
-      </c>
       <c r="J15" t="s">
         <v>8</v>
       </c>
@@ -1331,30 +1360,27 @@
         <v>200</v>
       </c>
       <c r="L15" t="s">
-        <v>88</v>
-      </c>
-      <c r="N15" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>175</v>
+        <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" t="s">
-        <v>96</v>
-      </c>
-      <c r="I17" t="s">
-        <v>96</v>
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" t="s">
+        <v>88</v>
       </c>
       <c r="J17" t="s">
         <v>8</v>
@@ -1363,30 +1389,88 @@
         <v>200</v>
       </c>
       <c r="L17" t="s">
-        <v>21</v>
+        <v>88</v>
+      </c>
+      <c r="N17" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B19" t="s">
-        <v>177</v>
+        <v>91</v>
       </c>
       <c r="C19" t="s">
-        <v>178</v>
+        <v>95</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>96</v>
+      </c>
+      <c r="I19" t="s">
+        <v>96</v>
+      </c>
+      <c r="J19" t="s">
+        <v>8</v>
       </c>
       <c r="K19">
         <v>200</v>
       </c>
       <c r="L19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21" t="s">
+        <v>178</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21">
+        <v>200</v>
+      </c>
+      <c r="L21" t="s">
         <v>22</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N21" t="s">
         <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" t="s">
+        <v>183</v>
+      </c>
+      <c r="D23" t="s">
+        <v>49</v>
+      </c>
+      <c r="J23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23">
+        <v>200</v>
+      </c>
+      <c r="L23" t="s">
+        <v>70</v>
+      </c>
+      <c r="N23" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1400,7 +1484,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G16" sqref="G16"/>
+      <selection pane="topRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,19 +1565,19 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="30" t="s">
         <v>8</v>
       </c>
       <c r="G6" t="s">
@@ -1516,11 +1600,11 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
-      <c r="F7" s="27"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="F7" s="30"/>
       <c r="K7">
         <v>500</v>
       </c>
@@ -1532,32 +1616,32 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="25" t="s">
+      <c r="G8" s="31"/>
+      <c r="H8" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="25" t="s">
+      <c r="J8" s="28" t="s">
         <v>8</v>
       </c>
       <c r="K8" s="3">
@@ -1574,16 +1658,16 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
       <c r="K9">
         <v>500</v>
       </c>
@@ -1598,16 +1682,16 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
       <c r="K10">
         <v>400</v>
       </c>
@@ -1622,16 +1706,16 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
       <c r="K11">
         <v>500</v>
       </c>
@@ -1646,16 +1730,16 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
       <c r="K12">
         <v>400</v>
       </c>
@@ -1957,7 +2041,7 @@
   <dimension ref="A3:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>